<commit_message>
att progress bar and program render
</commit_message>
<xml_diff>
--- a/Moedas.xlsx
+++ b/Moedas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Moedas</t>
   </si>
@@ -33,6 +33,15 @@
   </si>
   <si>
     <t>BTC</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>JPY</t>
+  </si>
+  <si>
+    <t>AUD</t>
   </si>
 </sst>
 </file>
@@ -359,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,7 +392,19 @@
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>